<commit_message>
korrekturen bis chapter 3 ohne diagramme
</commit_message>
<xml_diff>
--- a/5 - Metrics/str_1W_cpu_net.xlsx
+++ b/5 - Metrics/str_1W_cpu_net.xlsx
@@ -3519,11 +3519,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="324038032"/>
-        <c:axId val="324037488"/>
+        <c:axId val="820958272"/>
+        <c:axId val="820949024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="324038032"/>
+        <c:axId val="820958272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3565,7 +3565,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324037488"/>
+        <c:crossAx val="820949024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3573,7 +3573,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324037488"/>
+        <c:axId val="820949024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3624,7 +3624,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324038032"/>
+        <c:crossAx val="820958272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6630,11 +6630,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="324040208"/>
-        <c:axId val="324040752"/>
+        <c:axId val="820949568"/>
+        <c:axId val="820960992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="324040208"/>
+        <c:axId val="820949568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6676,7 +6676,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324040752"/>
+        <c:crossAx val="820960992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6684,7 +6684,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324040752"/>
+        <c:axId val="820960992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6736,7 +6736,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324040208"/>
+        <c:crossAx val="820949568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9742,11 +9742,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="238911536"/>
-        <c:axId val="238918608"/>
+        <c:axId val="820956640"/>
+        <c:axId val="820963168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="238911536"/>
+        <c:axId val="820956640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9788,7 +9788,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238918608"/>
+        <c:crossAx val="820963168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9796,7 +9796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238918608"/>
+        <c:axId val="820963168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -9848,7 +9848,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238911536"/>
+        <c:crossAx val="820956640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12847,11 +12847,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="323134880"/>
-        <c:axId val="323131616"/>
+        <c:axId val="820950112"/>
+        <c:axId val="820953920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="323134880"/>
+        <c:axId val="820950112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12893,7 +12893,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="323131616"/>
+        <c:crossAx val="820953920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12901,7 +12901,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="323131616"/>
+        <c:axId val="820953920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12952,7 +12952,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="323134880"/>
+        <c:crossAx val="820950112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15261,16 +15261,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15291,16 +15291,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>352426</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>409576</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15661,8 +15661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J466"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>